<commit_message>
update summary of AAPL logistic regression with rolling methods
</commit_message>
<xml_diff>
--- a/Market Intraday Momentum/AAPL_Repository_summary.xlsx
+++ b/Market Intraday Momentum/AAPL_Repository_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luzhang/Documents/GitHub/WrappingUp_Exploring_Intraday_Momentum/Market Intraday Momentum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B4B48A-0002-674F-ABC0-101ACD11984D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726C74C2-0FED-434D-AB91-DCCF516F4591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37400" yWindow="460" windowWidth="35840" windowHeight="19760" xr2:uid="{B6D1D89D-CA6C-7B42-999A-500C4E43312D}"/>
+    <workbookView xWindow="41220" yWindow="600" windowWidth="35840" windowHeight="19760" xr2:uid="{B6D1D89D-CA6C-7B42-999A-500C4E43312D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
   <si>
     <t>file name</t>
   </si>
@@ -182,6 +182,21 @@
   </si>
   <si>
     <t>K-fold cross validation</t>
+  </si>
+  <si>
+    <t>R file</t>
+  </si>
+  <si>
+    <t>AAPL_randomforest_raw_standardize_features.R</t>
+  </si>
+  <si>
+    <t>Logsitic Regression</t>
+  </si>
+  <si>
+    <t>AAPL_logisticRegression_raw_standardize_features.R</t>
+  </si>
+  <si>
+    <t>Without rolling validation</t>
   </si>
 </sst>
 </file>
@@ -240,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -274,17 +295,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -301,9 +316,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -317,13 +329,40 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -452,8 +491,8 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="588431" cy="281103"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -495,6 +534,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -537,7 +577,13 @@
                                 <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 </a:rPr>
-                                <m:t>92</m:t>
+                                <m:t>9</m:t>
+                              </m:r>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>2</m:t>
                               </m:r>
                             </m:e>
                             <m:e>
@@ -578,7 +624,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -648,8 +694,8 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="588430" cy="285719"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -691,6 +737,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -733,7 +780,13 @@
                                 <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 </a:rPr>
-                                <m:t>95</m:t>
+                                <m:t>9</m:t>
+                              </m:r>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>5</m:t>
                               </m:r>
                             </m:e>
                             <m:e>
@@ -774,7 +827,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -844,8 +897,8 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="588430" cy="282257"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -887,6 +940,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -929,7 +983,13 @@
                                 <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 </a:rPr>
-                                <m:t>72</m:t>
+                                <m:t>7</m:t>
+                              </m:r>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>2</m:t>
                               </m:r>
                             </m:e>
                             <m:e>
@@ -970,7 +1030,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -1040,8 +1100,8 @@
       <xdr:rowOff>260350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="660400" cy="282257"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1083,6 +1143,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1125,7 +1186,13 @@
                                 <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 </a:rPr>
-                                <m:t>90</m:t>
+                                <m:t>9</m:t>
+                              </m:r>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
                               </m:r>
                             </m:e>
                             <m:e>
@@ -1166,7 +1233,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1279,6 +1346,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1321,7 +1389,13 @@
                                 <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 </a:rPr>
-                                <m:t>348</m:t>
+                                <m:t>3</m:t>
+                              </m:r>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>48</m:t>
                               </m:r>
                             </m:e>
                             <m:e>
@@ -1404,6 +1478,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -1415,6 +1490,996 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>348&amp;77@94&amp;355)]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="588431" cy="281103"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65980D21-DC15-5146-BEB9-FD33C13DC885}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9283700" y="8616950"/>
+              <a:ext cx="588431" cy="281103"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:m>
+                          <m:mPr>
+                            <m:mcs>
+                              <m:mc>
+                                <m:mcPr>
+                                  <m:count m:val="2"/>
+                                  <m:mcJc m:val="center"/>
+                                </m:mcPr>
+                              </m:mc>
+                            </m:mcs>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:mPr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <m:rPr>
+                                  <m:brk m:alnAt="7"/>
+                                </m:rPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>98</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>17</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>19</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>86</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                        </m:m>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65980D21-DC15-5146-BEB9-FD33C13DC885}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9283700" y="8616950"/>
+              <a:ext cx="588431" cy="281103"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>[■8(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>98&amp;17@19&amp;86)]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="588430" cy="285719"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDDEB9A1-99E2-6B4B-AF30-F8C1D51CDB4F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9283700" y="8883650"/>
+              <a:ext cx="588430" cy="285719"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:m>
+                          <m:mPr>
+                            <m:mcs>
+                              <m:mc>
+                                <m:mcPr>
+                                  <m:count m:val="2"/>
+                                  <m:mcJc m:val="center"/>
+                                </m:mcPr>
+                              </m:mc>
+                            </m:mcs>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:mPr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <m:rPr>
+                                  <m:brk m:alnAt="7"/>
+                                </m:rPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>94</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>15</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>20</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>91</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                        </m:m>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDDEB9A1-99E2-6B4B-AF30-F8C1D51CDB4F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9283700" y="8883650"/>
+              <a:ext cx="588430" cy="285719"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>[■8(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>94&amp;15@20&amp;91)]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="588430" cy="282257"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A35D3C-AB02-4344-AC57-88DD2352F60A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9283700" y="10864850"/>
+              <a:ext cx="588430" cy="282257"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:m>
+                          <m:mPr>
+                            <m:mcs>
+                              <m:mc>
+                                <m:mcPr>
+                                  <m:count m:val="2"/>
+                                  <m:mcJc m:val="center"/>
+                                </m:mcPr>
+                              </m:mc>
+                            </m:mcs>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:mPr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <m:rPr>
+                                  <m:brk m:alnAt="7"/>
+                                </m:rPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>74</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>30</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>24</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>92</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                        </m:m>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A35D3C-AB02-4344-AC57-88DD2352F60A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9283700" y="10864850"/>
+              <a:ext cx="588430" cy="282257"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>[■8(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>74&amp;30@24&amp;92)]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>260350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="660400" cy="282257"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="TextBox 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07579FC4-6C2C-0342-A9B1-13DD4034E37A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9245600" y="9404350"/>
+              <a:ext cx="660400" cy="282257"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:m>
+                          <m:mPr>
+                            <m:mcs>
+                              <m:mc>
+                                <m:mcPr>
+                                  <m:count m:val="2"/>
+                                  <m:mcJc m:val="center"/>
+                                </m:mcPr>
+                              </m:mc>
+                            </m:mcs>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:mPr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <m:rPr>
+                                  <m:brk m:alnAt="7"/>
+                                </m:rPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>93</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>21</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>24</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>82</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                        </m:m>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="TextBox 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07579FC4-6C2C-0342-A9B1-13DD4034E37A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9245600" y="9404350"/>
+              <a:ext cx="660400" cy="282257"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>[■8(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>93&amp;21@24&amp;82)]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="744627" cy="285719"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="TextBox 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEB9CA6-ADE7-C046-9F40-5CD8D6FBC380}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="21894800" y="10598150"/>
+              <a:ext cx="744627" cy="285719"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:m>
+                          <m:mPr>
+                            <m:mcs>
+                              <m:mc>
+                                <m:mcPr>
+                                  <m:count m:val="2"/>
+                                  <m:mcJc m:val="center"/>
+                                </m:mcPr>
+                              </m:mc>
+                            </m:mcs>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:mPr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <m:rPr>
+                                  <m:brk m:alnAt="7"/>
+                                </m:rPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>359</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>74</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>83</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>358</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                        </m:m>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="TextBox 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEB9CA6-ADE7-C046-9F40-5CD8D6FBC380}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="21894800" y="10598150"/>
+              <a:ext cx="744627" cy="285719"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>[■8(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>359&amp;74@83&amp;358)]</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -1724,10 +2789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A83DF2-08A8-0B46-A3D8-10068C9D5CF0}">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1741,236 +2806,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="6" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="9" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="11"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="9" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="11"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="9" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="11"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="9" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="9" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="9" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="9" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="9" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="11"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="9" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="11"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="9" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="12"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1986,18 +3051,18 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.25">
@@ -2105,7 +3170,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="3" t="s">
         <v>34</v>
       </c>
       <c r="K22" s="1"/>
@@ -2133,7 +3198,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K24" s="1"/>
@@ -2164,106 +3229,110 @@
       <c r="J26" s="2"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:19" ht="22" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="9" t="s">
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="1"/>
-      <c r="M27" s="20" t="s">
+      <c r="K27" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="M27" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-    </row>
-    <row r="28" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+    </row>
+    <row r="28" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10" t="s">
+      <c r="I28" s="16"/>
+      <c r="J28" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="K28" s="1"/>
-      <c r="M28" s="14" t="s">
+      <c r="K28" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="N28" s="14" t="s">
+      <c r="N28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O28" s="14" t="s">
+      <c r="O28" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="P28" s="14" t="s">
+      <c r="P28" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="Q28" s="14" t="s">
+      <c r="Q28" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="R28" s="10" t="s">
+      <c r="R28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="S28" s="10"/>
-    </row>
-    <row r="29" spans="1:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="16" t="s">
+      <c r="S28" s="16"/>
+    </row>
+    <row r="29" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16"/>
+      <c r="B29" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="7">
         <v>0.81359999999999999</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="7">
         <v>0.84466019999999997</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="7">
         <v>0.8518519</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>0.78632480000000005</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>0.8177778</v>
       </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="1"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="23"/>
       <c r="M29">
         <v>0.80430000000000001</v>
       </c>
@@ -2279,114 +3348,347 @@
       <c r="Q29">
         <v>0.80276820000000004</v>
       </c>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-    </row>
-    <row r="30" spans="1:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="16" t="s">
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+    </row>
+    <row r="30" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="16"/>
+      <c r="B30" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="7">
         <v>0.84089999999999998</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="7">
         <v>0.84905660000000005</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="7">
         <v>0.8558559</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <v>0.83333330000000005</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>0.84444439999999998</v>
       </c>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="1:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="16" t="s">
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="23"/>
+    </row>
+    <row r="31" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="16"/>
+      <c r="B31" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="7">
         <v>0.77270000000000005</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="7">
         <v>0.80327870000000001</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>0.75</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>0.73469390000000001</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>0.74226800000000004</v>
       </c>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="1"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="23"/>
     </row>
     <row r="32" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="16"/>
+      <c r="B32" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="14">
         <v>0.78639999999999999</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="14">
         <v>0.80582520000000002</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="14">
         <v>0.81818179999999996</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="14">
         <v>0.76923079999999999</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="14">
         <v>0.79295150000000003</v>
       </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="15" t="s">
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="23"/>
+    </row>
+    <row r="33" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="15">
         <f>AVERAGE(C29:C32)</f>
         <v>0.8034</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="15">
         <f>AVERAGE(D29:D32)</f>
         <v>0.82570517500000007</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="15">
         <f>AVERAGE(E29:E32)</f>
         <v>0.81897240000000004</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F33" s="15">
         <f>AVERAGE(F29:F32)</f>
         <v>0.78089569999999997</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G33" s="15">
         <f>AVERAGE(G29:G32)</f>
         <v>0.79936042500000004</v>
       </c>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="10"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="23"/>
+    </row>
+    <row r="35" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K35" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+    </row>
+    <row r="36" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A36" s="16"/>
+      <c r="B36" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.83640000000000003</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0.83495149999999996</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0.85217390000000004</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.83760679999999998</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0.84482760000000001</v>
+      </c>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="23"/>
+      <c r="M36" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O36" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q36" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R36" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="S36" s="16"/>
+    </row>
+    <row r="37" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A37" s="16"/>
+      <c r="B37" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.84089999999999998</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0.85849059999999999</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0.86238530000000002</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0.8245614</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0.8430493</v>
+      </c>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="23"/>
+      <c r="M37">
+        <v>0.82040000000000002</v>
+      </c>
+      <c r="N37">
+        <v>0.82870370000000004</v>
+      </c>
+      <c r="O37">
+        <v>0.82909929999999998</v>
+      </c>
+      <c r="P37">
+        <v>0.81221719999999997</v>
+      </c>
+      <c r="Q37">
+        <v>0.82057139999999995</v>
+      </c>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+    </row>
+    <row r="38" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A38" s="16"/>
+      <c r="B38" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.75449999999999995</v>
+      </c>
+      <c r="D38" s="8">
+        <v>0.75409839999999995</v>
+      </c>
+      <c r="E38" s="8">
+        <v>0.71153849999999996</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0.75510200000000005</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0.73267329999999997</v>
+      </c>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="23"/>
+    </row>
+    <row r="39" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
+      <c r="B39" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="14">
+        <v>0.79549999999999998</v>
+      </c>
+      <c r="D39" s="14">
+        <v>0.7961165</v>
+      </c>
+      <c r="E39" s="14">
+        <v>0.81578949999999995</v>
+      </c>
+      <c r="F39" s="14">
+        <v>0.79487180000000002</v>
+      </c>
+      <c r="G39" s="14">
+        <v>0.80519479999999999</v>
+      </c>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="23"/>
+    </row>
+    <row r="40" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="15">
+        <f>AVERAGE(C36:C39)</f>
+        <v>0.80682500000000001</v>
+      </c>
+      <c r="D40" s="15">
+        <f>AVERAGE(D36:D39)</f>
+        <v>0.81091424999999995</v>
+      </c>
+      <c r="E40" s="15">
+        <f>AVERAGE(E36:E39)</f>
+        <v>0.81047179999999996</v>
+      </c>
+      <c r="F40" s="15">
+        <f>AVERAGE(F36:F39)</f>
+        <v>0.80303550000000001</v>
+      </c>
+      <c r="G40" s="15">
+        <f>AVERAGE(G36:G39)</f>
+        <v>0.80643624999999997</v>
+      </c>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="39">
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="M35:S35"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:J40"/>
+    <mergeCell ref="K35:K40"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B4:I4"/>
     <mergeCell ref="R28:S28"/>
     <mergeCell ref="M27:S27"/>
     <mergeCell ref="R29:S29"/>
@@ -2400,19 +3702,7 @@
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="K28:K33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>